<commit_message>
complete export schedule teacher (example data)
</commit_message>
<xml_diff>
--- a/studMin/TemplateExcel/schedule_teacher.xlsx
+++ b/studMin/TemplateExcel/schedule_teacher.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiet\source\repos\WindowsFormsApp1\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiet\source\repos\studMin\studMin\TemplateExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447E7D29-B2DA-41F9-93D4-AB237DDD8747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100EE841-A265-4B11-A737-0EF358AC6AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -297,6 +297,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -312,22 +324,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -613,7 +613,7 @@
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -621,7 +621,7 @@
     <col min="1" max="1" width="6.796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.06640625" style="14"/>
+    <col min="4" max="4" width="26.59765625" style="7" customWidth="1"/>
     <col min="5" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
@@ -645,916 +645,918 @@
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="14">
         <v>1</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="16"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="11">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="15">
         <v>2</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="16"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="11">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="15">
         <v>3</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="11">
-        <v>4</v>
-      </c>
-      <c r="D10" s="16"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="15">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="16"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="11">
-        <v>5</v>
-      </c>
-      <c r="D12" s="16"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="15">
+        <v>5</v>
+      </c>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="16"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" s="8"/>
-      <c r="B14" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="10">
+      <c r="A14" s="12"/>
+      <c r="B14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="14">
         <v>1</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="16"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="11">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="15">
         <v>2</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="16"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="11">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="15">
         <v>3</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="11">
-        <v>4</v>
-      </c>
-      <c r="D20" s="16"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="15">
+        <v>4</v>
+      </c>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="16"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="11">
-        <v>5</v>
-      </c>
-      <c r="D22" s="16"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="15">
+        <v>5</v>
+      </c>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="17"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="10">
+      <c r="B24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="14">
         <v>1</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="16"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="11">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="15">
         <v>2</v>
       </c>
-      <c r="D26" s="16"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="16"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="11">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="15">
         <v>3</v>
       </c>
-      <c r="D28" s="16"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="16"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="11">
-        <v>4</v>
-      </c>
-      <c r="D30" s="16"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="15">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="16"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="11">
-        <v>5</v>
-      </c>
-      <c r="D32" s="16"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="15">
+        <v>5</v>
+      </c>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="16"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="10">
+      <c r="A34" s="12"/>
+      <c r="B34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="14">
         <v>1</v>
       </c>
-      <c r="D34" s="15"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="16"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="11">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="15">
         <v>2</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="16"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="11">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="15">
         <v>3</v>
       </c>
-      <c r="D38" s="16"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="16"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="11">
-        <v>4</v>
-      </c>
-      <c r="D40" s="16"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="15">
+        <v>4</v>
+      </c>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="16"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="11">
-        <v>5</v>
-      </c>
-      <c r="D42" s="16"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="15">
+        <v>5</v>
+      </c>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="17"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="10">
+      <c r="B44" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="14">
         <v>1</v>
       </c>
-      <c r="D44" s="15"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="16"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="11">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="15">
         <v>2</v>
       </c>
-      <c r="D46" s="16"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="16"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="11">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="15">
         <v>3</v>
       </c>
-      <c r="D48" s="16"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="16"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="11">
-        <v>4</v>
-      </c>
-      <c r="D50" s="16"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="15">
+        <v>4</v>
+      </c>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="16"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="11">
-        <v>5</v>
-      </c>
-      <c r="D52" s="16"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="15">
+        <v>5</v>
+      </c>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="16"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A54" s="8"/>
-      <c r="B54" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="10">
+      <c r="A54" s="12"/>
+      <c r="B54" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="14">
         <v>1</v>
       </c>
-      <c r="D54" s="15"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="16"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="11">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="15">
         <v>2</v>
       </c>
-      <c r="D56" s="16"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="16"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="11">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="15">
         <v>3</v>
       </c>
-      <c r="D58" s="16"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="16"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="11">
-        <v>4</v>
-      </c>
-      <c r="D60" s="16"/>
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="15">
+        <v>4</v>
+      </c>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="16"/>
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="9"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="11">
-        <v>5</v>
-      </c>
-      <c r="D62" s="16"/>
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="15">
+        <v>5</v>
+      </c>
+      <c r="D62" s="9"/>
     </row>
     <row r="63" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="17"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" s="10">
+      <c r="B64" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="14">
         <v>1</v>
       </c>
-      <c r="D64" s="15"/>
+      <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="16"/>
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="9"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="11">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="15">
         <v>2</v>
       </c>
-      <c r="D66" s="16"/>
+      <c r="D66" s="9"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A67" s="8"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="16"/>
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="9"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="11">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="15">
         <v>3</v>
       </c>
-      <c r="D68" s="16"/>
+      <c r="D68" s="9"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="16"/>
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="9"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="11">
-        <v>4</v>
-      </c>
-      <c r="D70" s="16"/>
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="15">
+        <v>4</v>
+      </c>
+      <c r="D70" s="9"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="16"/>
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="9"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A72" s="8"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="11">
-        <v>5</v>
-      </c>
-      <c r="D72" s="16"/>
+      <c r="A72" s="12"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="15">
+        <v>5</v>
+      </c>
+      <c r="D72" s="9"/>
     </row>
     <row r="73" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="16"/>
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="9"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A74" s="8"/>
-      <c r="B74" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="10">
+      <c r="A74" s="12"/>
+      <c r="B74" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="14">
         <v>1</v>
       </c>
-      <c r="D74" s="15"/>
+      <c r="D74" s="8"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A75" s="8"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="16"/>
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="9"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="11">
+      <c r="A76" s="12"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="15">
         <v>2</v>
       </c>
-      <c r="D76" s="16"/>
+      <c r="D76" s="9"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A77" s="8"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="16"/>
+      <c r="A77" s="12"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="9"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="11">
+      <c r="A78" s="12"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="15">
         <v>3</v>
       </c>
-      <c r="D78" s="16"/>
+      <c r="D78" s="9"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="16"/>
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="9"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A80" s="8"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="11">
-        <v>4</v>
-      </c>
-      <c r="D80" s="16"/>
+      <c r="A80" s="12"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="15">
+        <v>4</v>
+      </c>
+      <c r="D80" s="9"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A81" s="8"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="16"/>
+      <c r="A81" s="12"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="9"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A82" s="8"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="11">
-        <v>5</v>
-      </c>
-      <c r="D82" s="16"/>
+      <c r="A82" s="12"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="15">
+        <v>5</v>
+      </c>
+      <c r="D82" s="9"/>
     </row>
     <row r="83" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="17"/>
+      <c r="A83" s="13"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="10"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B84" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C84" s="10">
+      <c r="B84" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="14">
         <v>1</v>
       </c>
-      <c r="D84" s="15"/>
+      <c r="D84" s="8"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="16"/>
+      <c r="A85" s="12"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="9"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="11">
+      <c r="A86" s="12"/>
+      <c r="B86" s="12"/>
+      <c r="C86" s="15">
         <v>2</v>
       </c>
-      <c r="D86" s="16"/>
+      <c r="D86" s="9"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A87" s="8"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="16"/>
+      <c r="A87" s="12"/>
+      <c r="B87" s="12"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="9"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A88" s="8"/>
-      <c r="B88" s="8"/>
-      <c r="C88" s="11">
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="15">
         <v>3</v>
       </c>
-      <c r="D88" s="16"/>
+      <c r="D88" s="9"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A89" s="8"/>
-      <c r="B89" s="8"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="16"/>
+      <c r="A89" s="12"/>
+      <c r="B89" s="12"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="9"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A90" s="8"/>
-      <c r="B90" s="8"/>
-      <c r="C90" s="11">
-        <v>4</v>
-      </c>
-      <c r="D90" s="16"/>
+      <c r="A90" s="12"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="15">
+        <v>4</v>
+      </c>
+      <c r="D90" s="9"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A91" s="8"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="16"/>
+      <c r="A91" s="12"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="9"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A92" s="8"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="11">
-        <v>5</v>
-      </c>
-      <c r="D92" s="16"/>
+      <c r="A92" s="12"/>
+      <c r="B92" s="12"/>
+      <c r="C92" s="15">
+        <v>5</v>
+      </c>
+      <c r="D92" s="9"/>
     </row>
     <row r="93" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="8"/>
-      <c r="B93" s="8"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="16"/>
+      <c r="A93" s="12"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="9"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A94" s="8"/>
-      <c r="B94" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="10">
+      <c r="A94" s="12"/>
+      <c r="B94" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="14">
         <v>1</v>
       </c>
-      <c r="D94" s="15"/>
+      <c r="D94" s="8"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A95" s="8"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="16"/>
+      <c r="A95" s="12"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="9"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A96" s="8"/>
-      <c r="B96" s="8"/>
-      <c r="C96" s="11">
+      <c r="A96" s="12"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="15">
         <v>2</v>
       </c>
-      <c r="D96" s="16"/>
+      <c r="D96" s="9"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A97" s="8"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="16"/>
+      <c r="A97" s="12"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="15"/>
+      <c r="D97" s="9"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A98" s="8"/>
-      <c r="B98" s="8"/>
-      <c r="C98" s="11">
+      <c r="A98" s="12"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="15">
         <v>3</v>
       </c>
-      <c r="D98" s="16"/>
+      <c r="D98" s="9"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A99" s="8"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="11"/>
-      <c r="D99" s="16"/>
+      <c r="A99" s="12"/>
+      <c r="B99" s="12"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="9"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A100" s="8"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="11">
-        <v>4</v>
-      </c>
-      <c r="D100" s="16"/>
+      <c r="A100" s="12"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="15">
+        <v>4</v>
+      </c>
+      <c r="D100" s="9"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A101" s="8"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="16"/>
+      <c r="A101" s="12"/>
+      <c r="B101" s="12"/>
+      <c r="C101" s="15"/>
+      <c r="D101" s="9"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A102" s="8"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="11">
-        <v>5</v>
-      </c>
-      <c r="D102" s="16"/>
+      <c r="A102" s="12"/>
+      <c r="B102" s="12"/>
+      <c r="C102" s="15">
+        <v>5</v>
+      </c>
+      <c r="D102" s="9"/>
     </row>
     <row r="103" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="9"/>
-      <c r="B103" s="9"/>
-      <c r="C103" s="12"/>
-      <c r="D103" s="17"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="10"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A104" s="7" t="s">
+      <c r="A104" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B104" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C104" s="10">
+      <c r="B104" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C104" s="14">
         <v>1</v>
       </c>
-      <c r="D104" s="15"/>
+      <c r="D104" s="8"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A105" s="8"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="16"/>
+      <c r="A105" s="12"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="15"/>
+      <c r="D105" s="9"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A106" s="8"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="11">
+      <c r="A106" s="12"/>
+      <c r="B106" s="12"/>
+      <c r="C106" s="15">
         <v>2</v>
       </c>
-      <c r="D106" s="16"/>
+      <c r="D106" s="9"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A107" s="8"/>
-      <c r="B107" s="8"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="16"/>
+      <c r="A107" s="12"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="9"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A108" s="8"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="11">
+      <c r="A108" s="12"/>
+      <c r="B108" s="12"/>
+      <c r="C108" s="15">
         <v>3</v>
       </c>
-      <c r="D108" s="16"/>
+      <c r="D108" s="9"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A109" s="8"/>
-      <c r="B109" s="8"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="16"/>
+      <c r="A109" s="12"/>
+      <c r="B109" s="12"/>
+      <c r="C109" s="15"/>
+      <c r="D109" s="9"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A110" s="8"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="11">
-        <v>4</v>
-      </c>
-      <c r="D110" s="16"/>
+      <c r="A110" s="12"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="15">
+        <v>4</v>
+      </c>
+      <c r="D110" s="9"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A111" s="8"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="16"/>
+      <c r="A111" s="12"/>
+      <c r="B111" s="12"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="9"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A112" s="8"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="11">
-        <v>5</v>
-      </c>
-      <c r="D112" s="16"/>
+      <c r="A112" s="12"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="15">
+        <v>5</v>
+      </c>
+      <c r="D112" s="9"/>
     </row>
     <row r="113" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A113" s="8"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="13"/>
-      <c r="D113" s="16"/>
+      <c r="A113" s="12"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="9"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A114" s="8"/>
-      <c r="B114" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" s="10">
+      <c r="A114" s="12"/>
+      <c r="B114" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="14">
         <v>1</v>
       </c>
-      <c r="D114" s="15"/>
+      <c r="D114" s="8"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A115" s="8"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="16"/>
+      <c r="A115" s="12"/>
+      <c r="B115" s="12"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="9"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A116" s="8"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="11">
+      <c r="A116" s="12"/>
+      <c r="B116" s="12"/>
+      <c r="C116" s="15">
         <v>2</v>
       </c>
-      <c r="D116" s="16"/>
+      <c r="D116" s="9"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A117" s="8"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="16"/>
+      <c r="A117" s="12"/>
+      <c r="B117" s="12"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="9"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A118" s="8"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="11">
+      <c r="A118" s="12"/>
+      <c r="B118" s="12"/>
+      <c r="C118" s="15">
         <v>3</v>
       </c>
-      <c r="D118" s="16"/>
+      <c r="D118" s="9"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A119" s="8"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="11"/>
-      <c r="D119" s="16"/>
+      <c r="A119" s="12"/>
+      <c r="B119" s="12"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="9"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A120" s="8"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="11">
-        <v>4</v>
-      </c>
-      <c r="D120" s="16"/>
+      <c r="A120" s="12"/>
+      <c r="B120" s="12"/>
+      <c r="C120" s="15">
+        <v>4</v>
+      </c>
+      <c r="D120" s="9"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A121" s="8"/>
-      <c r="B121" s="8"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="16"/>
+      <c r="A121" s="12"/>
+      <c r="B121" s="12"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="9"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A122" s="8"/>
-      <c r="B122" s="8"/>
-      <c r="C122" s="11">
-        <v>5</v>
-      </c>
-      <c r="D122" s="16"/>
+      <c r="A122" s="12"/>
+      <c r="B122" s="12"/>
+      <c r="C122" s="15">
+        <v>5</v>
+      </c>
+      <c r="D122" s="9"/>
     </row>
     <row r="123" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A123" s="9"/>
-      <c r="B123" s="9"/>
-      <c r="C123" s="12"/>
-      <c r="D123" s="17"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="17"/>
+      <c r="D123" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="A4:A23"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="B14:B23"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A24:A43"/>
-    <mergeCell ref="B24:B33"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B34:B43"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="A84:A103"/>
+    <mergeCell ref="B84:B93"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="B94:B103"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="C102:C103"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="A104:A123"/>
+    <mergeCell ref="B104:B113"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="B114:B123"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="B74:B83"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C82:C83"/>
     <mergeCell ref="A44:A63"/>
     <mergeCell ref="B44:B53"/>
     <mergeCell ref="C44:C45"/>
@@ -1571,38 +1573,36 @@
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="C64:C65"/>
     <mergeCell ref="C46:C47"/>
-    <mergeCell ref="B74:B83"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="A104:A123"/>
-    <mergeCell ref="B104:B113"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="C110:C111"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="A84:A103"/>
-    <mergeCell ref="B84:B93"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="B94:B103"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="B114:B123"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="A24:A43"/>
+    <mergeCell ref="B24:B33"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B34:B43"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="B14:B23"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="A4:A23"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>